<commit_message>
update electricity generation data files
</commit_message>
<xml_diff>
--- a/data/Table_7.2a_Electricity_Net_Generation__Total_(All_Sectors).xlsx
+++ b/data/Table_7.2a_Electricity_Net_Generation__Total_(All_Sectors).xlsx
@@ -21,13 +21,13 @@
     <t>U.S. Energy Information Administration</t>
   </si>
   <si>
-    <t>August 2018 Monthly Energy Review</t>
+    <t>July 2020 Monthly Energy Review</t>
   </si>
   <si>
-    <t>Release Date: August 28, 2018</t>
+    <t>Release Date: July 28, 2020</t>
   </si>
   <si>
-    <t>Next Update: September 25, 2018</t>
+    <t>Next Update: August 26, 2020</t>
   </si>
   <si>
     <t>Table 7.2a Electricity Net Generation: Total (All Sectors)</t>
@@ -72,7 +72,7 @@
     <t>Electricity Net Generation From Wind, All Sectors</t>
   </si>
   <si>
-    <t>Electricity Net Generation Total, All Sectors</t>
+    <t>Electricity Net Generation Total (including from sources not shown), All Sectors</t>
   </si>
   <si>
     <t>(Million Kilowatthours)</t>
@@ -488,7 +488,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N557"/>
+  <dimension ref="A1:N580"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A13" sqref="A13"/>
@@ -509,7 +509,7 @@
     <col min="11" max="11" width="59.842529" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="54.558105" bestFit="true" customWidth="true" style="0"/>
     <col min="13" max="13" width="53.415527" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="49.130859" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="86.693115" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -23866,16 +23866,16 @@
         <v>42736</v>
       </c>
       <c r="B541">
-        <v>115501.399</v>
+        <v>115332.808</v>
       </c>
       <c r="C541">
-        <v>2073.747</v>
+        <v>2045.775</v>
       </c>
       <c r="D541">
-        <v>91446.529</v>
+        <v>95572.229</v>
       </c>
       <c r="E541">
-        <v>1120.301</v>
+        <v>1046.564</v>
       </c>
       <c r="F541">
         <v>73120.612</v>
@@ -23884,25 +23884,25 @@
         <v>-435.366</v>
       </c>
       <c r="H541">
-        <v>27853.164</v>
+        <v>26627.881</v>
       </c>
       <c r="I541">
-        <v>3589.003</v>
+        <v>3502.178</v>
       </c>
       <c r="J541">
-        <v>1863.336</v>
+        <v>1897.391</v>
       </c>
       <c r="K541">
-        <v>1399.462</v>
+        <v>1406.967</v>
       </c>
       <c r="L541">
-        <v>2151.925</v>
+        <v>2323.986</v>
       </c>
       <c r="M541">
-        <v>20748.608</v>
+        <v>20798.771</v>
       </c>
       <c r="N541">
-        <v>341518.167</v>
+        <v>344332.034</v>
       </c>
     </row>
     <row r="542" spans="1:14">
@@ -23910,16 +23910,16 @@
         <v>42767</v>
       </c>
       <c r="B542">
-        <v>86872.774</v>
+        <v>86822.19</v>
       </c>
       <c r="C542">
-        <v>1591.822</v>
+        <v>1591.883</v>
       </c>
       <c r="D542">
-        <v>81040.212</v>
+        <v>82767.651</v>
       </c>
       <c r="E542">
-        <v>1190.57</v>
+        <v>977.644</v>
       </c>
       <c r="F542">
         <v>63560.371</v>
@@ -23928,25 +23928,25 @@
         <v>-507.911</v>
       </c>
       <c r="H542">
-        <v>24541.655</v>
+        <v>23881.765</v>
       </c>
       <c r="I542">
-        <v>3404.916</v>
+        <v>3185.521</v>
       </c>
       <c r="J542">
-        <v>1646.656</v>
+        <v>1697.118</v>
       </c>
       <c r="K542">
-        <v>1241.317</v>
+        <v>1238.872</v>
       </c>
       <c r="L542">
-        <v>2496.672</v>
+        <v>2751.199</v>
       </c>
       <c r="M542">
-        <v>22228.202</v>
+        <v>22091.109</v>
       </c>
       <c r="N542">
-        <v>290296.836</v>
+        <v>291049.672</v>
       </c>
     </row>
     <row r="543" spans="1:14">
@@ -23954,16 +23954,16 @@
         <v>42795</v>
       </c>
       <c r="B543">
-        <v>89426.812</v>
+        <v>89364.62</v>
       </c>
       <c r="C543">
-        <v>1686.401</v>
+        <v>1655.495</v>
       </c>
       <c r="D543">
-        <v>94707.94</v>
+        <v>95073.662</v>
       </c>
       <c r="E543">
-        <v>1257.498</v>
+        <v>1060.248</v>
       </c>
       <c r="F543">
         <v>65093.2</v>
@@ -23972,25 +23972,25 @@
         <v>-521.035</v>
       </c>
       <c r="H543">
-        <v>30220.915</v>
+        <v>29613.195</v>
       </c>
       <c r="I543">
-        <v>3661.934</v>
+        <v>3455.802</v>
       </c>
       <c r="J543">
-        <v>1759.981</v>
+        <v>1847.569</v>
       </c>
       <c r="K543">
-        <v>1379.83</v>
+        <v>1387.185</v>
       </c>
       <c r="L543">
-        <v>4432.648</v>
+        <v>4514.085</v>
       </c>
       <c r="M543">
-        <v>26132.697</v>
+        <v>25730.617</v>
       </c>
       <c r="N543">
-        <v>320290.909</v>
+        <v>319335.755</v>
       </c>
     </row>
     <row r="544" spans="1:14">
@@ -23998,16 +23998,16 @@
         <v>42826</v>
       </c>
       <c r="B544">
-        <v>81533.004</v>
+        <v>81335.313</v>
       </c>
       <c r="C544">
-        <v>1287.501</v>
+        <v>1290.668</v>
       </c>
       <c r="D544">
-        <v>86178.096</v>
+        <v>88455.101</v>
       </c>
       <c r="E544">
-        <v>1156.858</v>
+        <v>1001.36</v>
       </c>
       <c r="F544">
         <v>56743.352</v>
@@ -24016,25 +24016,25 @@
         <v>-438.729</v>
       </c>
       <c r="H544">
-        <v>29319.643</v>
+        <v>29409.466</v>
       </c>
       <c r="I544">
-        <v>3372.73</v>
+        <v>3146.376</v>
       </c>
       <c r="J544">
-        <v>1671.335</v>
+        <v>1741.69</v>
       </c>
       <c r="K544">
-        <v>1357.349</v>
+        <v>1341.221</v>
       </c>
       <c r="L544">
-        <v>4774.175</v>
+        <v>4906.678</v>
       </c>
       <c r="M544">
-        <v>25752.898</v>
+        <v>25377.943</v>
       </c>
       <c r="N544">
-        <v>293752.39</v>
+        <v>295360.591</v>
       </c>
     </row>
     <row r="545" spans="1:14">
@@ -24042,16 +24042,16 @@
         <v>42856</v>
       </c>
       <c r="B545">
-        <v>92880.558</v>
+        <v>92776.541</v>
       </c>
       <c r="C545">
-        <v>1773.776</v>
+        <v>1816.995</v>
       </c>
       <c r="D545">
-        <v>96777.016</v>
+        <v>98019.311</v>
       </c>
       <c r="E545">
-        <v>1181.702</v>
+        <v>1055.752</v>
       </c>
       <c r="F545">
         <v>61312.753</v>
@@ -24060,25 +24060,25 @@
         <v>-423.168</v>
       </c>
       <c r="H545">
-        <v>32177</v>
+        <v>32607.115</v>
       </c>
       <c r="I545">
-        <v>3437.855</v>
+        <v>3188.454</v>
       </c>
       <c r="J545">
-        <v>1743.261</v>
+        <v>1849.796</v>
       </c>
       <c r="K545">
-        <v>1295.062</v>
+        <v>1301.858</v>
       </c>
       <c r="L545">
-        <v>5766.305</v>
+        <v>5785.027</v>
       </c>
       <c r="M545">
-        <v>22641.882</v>
+        <v>23067.639</v>
       </c>
       <c r="N545">
-        <v>321645.178</v>
+        <v>323446.738</v>
       </c>
     </row>
     <row r="546" spans="1:14">
@@ -24086,16 +24086,16 @@
         <v>42887</v>
       </c>
       <c r="B546">
-        <v>107727.822</v>
+        <v>107508.322</v>
       </c>
       <c r="C546">
-        <v>1879.552</v>
+        <v>1892.864</v>
       </c>
       <c r="D546">
-        <v>116060.925</v>
+        <v>117235.701</v>
       </c>
       <c r="E546">
-        <v>1210.947</v>
+        <v>992.976</v>
       </c>
       <c r="F546">
         <v>67010.782</v>
@@ -24104,25 +24104,25 @@
         <v>-567.516</v>
       </c>
       <c r="H546">
-        <v>30423.839</v>
+        <v>30575.296</v>
       </c>
       <c r="I546">
-        <v>3624.557</v>
+        <v>3437.011</v>
       </c>
       <c r="J546">
-        <v>1695.427</v>
+        <v>1796.52</v>
       </c>
       <c r="K546">
-        <v>1264.744</v>
+        <v>1283.75</v>
       </c>
       <c r="L546">
-        <v>6252.324</v>
+        <v>6115.379</v>
       </c>
       <c r="M546">
-        <v>19711.086</v>
+        <v>20141.747</v>
       </c>
       <c r="N546">
-        <v>357390.443</v>
+        <v>358522.007</v>
       </c>
     </row>
     <row r="547" spans="1:14">
@@ -24130,16 +24130,16 @@
         <v>42917</v>
       </c>
       <c r="B547">
-        <v>127958.904</v>
+        <v>127697.82</v>
       </c>
       <c r="C547">
-        <v>1746.97</v>
+        <v>1809.594</v>
       </c>
       <c r="D547">
-        <v>144719.63</v>
+        <v>146929.439</v>
       </c>
       <c r="E547">
-        <v>1260.614</v>
+        <v>1047.488</v>
       </c>
       <c r="F547">
         <v>71314.219</v>
@@ -24148,25 +24148,25 @@
         <v>-759.494</v>
       </c>
       <c r="H547">
-        <v>25745.023</v>
+        <v>26598.247</v>
       </c>
       <c r="I547">
-        <v>3921.756</v>
+        <v>3702.896</v>
       </c>
       <c r="J547">
-        <v>1759.769</v>
+        <v>1823.779</v>
       </c>
       <c r="K547">
-        <v>1367.808</v>
+        <v>1372.704</v>
       </c>
       <c r="L547">
-        <v>5504.588</v>
+        <v>5569.106</v>
       </c>
       <c r="M547">
-        <v>15764.963</v>
+        <v>16119.996</v>
       </c>
       <c r="N547">
-        <v>401509.614</v>
+        <v>404432.474</v>
       </c>
     </row>
     <row r="548" spans="1:14">
@@ -24174,16 +24174,16 @@
         <v>42948</v>
       </c>
       <c r="B548">
-        <v>119780.304</v>
+        <v>119488.385</v>
       </c>
       <c r="C548">
-        <v>1724.104</v>
+        <v>1733.107</v>
       </c>
       <c r="D548">
-        <v>139609.587</v>
+        <v>141201.138</v>
       </c>
       <c r="E548">
-        <v>1320.665</v>
+        <v>1133.26</v>
       </c>
       <c r="F548">
         <v>72384.218</v>
@@ -24192,25 +24192,25 @@
         <v>-638.234</v>
       </c>
       <c r="H548">
-        <v>21240.745</v>
+        <v>22033.856</v>
       </c>
       <c r="I548">
-        <v>3879.728</v>
+        <v>3750.568</v>
       </c>
       <c r="J548">
-        <v>1775.191</v>
+        <v>1824.891</v>
       </c>
       <c r="K548">
-        <v>1357.042</v>
+        <v>1362.996</v>
       </c>
       <c r="L548">
-        <v>5401.318</v>
+        <v>5368.537</v>
       </c>
       <c r="M548">
-        <v>13088.831</v>
+        <v>13878.848</v>
       </c>
       <c r="N548">
-        <v>382140.08</v>
+        <v>384738.58</v>
       </c>
     </row>
     <row r="549" spans="1:14">
@@ -24218,16 +24218,16 @@
         <v>42979</v>
       </c>
       <c r="B549">
-        <v>98404.05</v>
+        <v>98202.046</v>
       </c>
       <c r="C549">
-        <v>1664.991</v>
+        <v>1643.037</v>
       </c>
       <c r="D549">
-        <v>116728.411</v>
+        <v>118035.852</v>
       </c>
       <c r="E549">
-        <v>1120.29</v>
+        <v>1059.443</v>
       </c>
       <c r="F549">
         <v>68097.918</v>
@@ -24236,25 +24236,25 @@
         <v>-606.081</v>
       </c>
       <c r="H549">
-        <v>18964.595</v>
+        <v>19151.755</v>
       </c>
       <c r="I549">
-        <v>3403.918</v>
+        <v>3291.751</v>
       </c>
       <c r="J549">
-        <v>1649.453</v>
+        <v>1702.546</v>
       </c>
       <c r="K549">
-        <v>1325.436</v>
+        <v>1331.503</v>
       </c>
       <c r="L549">
-        <v>5167.765</v>
+        <v>5059.441</v>
       </c>
       <c r="M549">
-        <v>17268.055</v>
+        <v>17911.775</v>
       </c>
       <c r="N549">
-        <v>334218.636</v>
+        <v>335914.91</v>
       </c>
     </row>
     <row r="550" spans="1:14">
@@ -24262,16 +24262,16 @@
         <v>43009</v>
       </c>
       <c r="B550">
-        <v>90087.106</v>
+        <v>89775.524</v>
       </c>
       <c r="C550">
-        <v>1533.369</v>
+        <v>1545.345</v>
       </c>
       <c r="D550">
-        <v>106866.996</v>
+        <v>106826.275</v>
       </c>
       <c r="E550">
-        <v>1013.786</v>
+        <v>998.167</v>
       </c>
       <c r="F550">
         <v>65994.785</v>
@@ -24280,25 +24280,25 @@
         <v>-462.982</v>
       </c>
       <c r="H550">
-        <v>17210.514</v>
+        <v>17698.179</v>
       </c>
       <c r="I550">
-        <v>3569.268</v>
+        <v>3303.263</v>
       </c>
       <c r="J550">
-        <v>1692.642</v>
+        <v>1727.853</v>
       </c>
       <c r="K550">
-        <v>1260.904</v>
+        <v>1214.124</v>
       </c>
       <c r="L550">
-        <v>4830.2</v>
+        <v>4649.673</v>
       </c>
       <c r="M550">
-        <v>24821.2</v>
+        <v>24368.703</v>
       </c>
       <c r="N550">
-        <v>319443.133</v>
+        <v>318669.649</v>
       </c>
     </row>
     <row r="551" spans="1:14">
@@ -24306,16 +24306,16 @@
         <v>43040</v>
       </c>
       <c r="B551">
-        <v>91150.728</v>
+        <v>90986.339</v>
       </c>
       <c r="C551">
-        <v>1615.728</v>
+        <v>1669.858</v>
       </c>
       <c r="D551">
-        <v>92584.737</v>
+        <v>94928.341</v>
       </c>
       <c r="E551">
-        <v>1198.178</v>
+        <v>1001.041</v>
       </c>
       <c r="F551">
         <v>66617.853</v>
@@ -24324,25 +24324,25 @@
         <v>-478.107</v>
       </c>
       <c r="H551">
-        <v>19840.471</v>
+        <v>19888.334</v>
       </c>
       <c r="I551">
-        <v>3559.668</v>
+        <v>3426.085</v>
       </c>
       <c r="J551">
-        <v>1720.927</v>
+        <v>1804.841</v>
       </c>
       <c r="K551">
-        <v>1334.106</v>
+        <v>1304.684</v>
       </c>
       <c r="L551">
-        <v>3120.418</v>
+        <v>3208.749</v>
       </c>
       <c r="M551">
-        <v>23320.136</v>
+        <v>22614.867</v>
       </c>
       <c r="N551">
-        <v>306659.705</v>
+        <v>308052.342</v>
       </c>
     </row>
     <row r="552" spans="1:14">
@@ -24350,16 +24350,16 @@
         <v>43070</v>
       </c>
       <c r="B552">
-        <v>106577.846</v>
+        <v>106545.367</v>
       </c>
       <c r="C552">
-        <v>2513.211</v>
+        <v>2695.323</v>
       </c>
       <c r="D552">
-        <v>106144.086</v>
+        <v>111397.792</v>
       </c>
       <c r="E552">
-        <v>1127.457</v>
+        <v>1095.024</v>
       </c>
       <c r="F552">
         <v>73699.572</v>
@@ -24368,25 +24368,25 @@
         <v>-655.925</v>
       </c>
       <c r="H552">
-        <v>22506.938</v>
+        <v>22247.842</v>
       </c>
       <c r="I552">
-        <v>3858.586</v>
+        <v>3733.613</v>
       </c>
       <c r="J552">
-        <v>1794.638</v>
+        <v>1895.898</v>
       </c>
       <c r="K552">
-        <v>1392.982</v>
+        <v>1380.91</v>
       </c>
       <c r="L552">
-        <v>3059.442</v>
+        <v>3035.005</v>
       </c>
       <c r="M552">
-        <v>22775.781</v>
+        <v>22200.681</v>
       </c>
       <c r="N552">
-        <v>345939.372</v>
+        <v>350415.808</v>
       </c>
     </row>
     <row r="553" spans="1:14">
@@ -24394,16 +24394,16 @@
         <v>43101</v>
       </c>
       <c r="B553">
-        <v>118695.621</v>
+        <v>119284.115</v>
       </c>
       <c r="C553">
-        <v>6135.191</v>
+        <v>6519.897</v>
       </c>
       <c r="D553">
-        <v>109601.065</v>
+        <v>110292.909</v>
       </c>
       <c r="E553">
-        <v>1060.109</v>
+        <v>1096.622</v>
       </c>
       <c r="F553">
         <v>74649.04</v>
@@ -24412,25 +24412,25 @@
         <v>-547.331</v>
       </c>
       <c r="H553">
-        <v>25422.001</v>
+        <v>25064.077</v>
       </c>
       <c r="I553">
-        <v>3846.61</v>
+        <v>3685.99</v>
       </c>
       <c r="J553">
-        <v>1766.929</v>
+        <v>1816.607</v>
       </c>
       <c r="K553">
-        <v>1373.357</v>
+        <v>1341.307</v>
       </c>
       <c r="L553">
-        <v>3262.036</v>
+        <v>3318.975</v>
       </c>
       <c r="M553">
-        <v>26833.64</v>
+        <v>25598.822</v>
       </c>
       <c r="N553">
-        <v>373213.093</v>
+        <v>373230.28</v>
       </c>
     </row>
     <row r="554" spans="1:14">
@@ -24438,16 +24438,16 @@
         <v>43132</v>
       </c>
       <c r="B554">
-        <v>82050.779</v>
+        <v>82050.182</v>
       </c>
       <c r="C554">
-        <v>1509.339</v>
+        <v>1557.624</v>
       </c>
       <c r="D554">
-        <v>96317.327</v>
+        <v>98511.852</v>
       </c>
       <c r="E554">
-        <v>1092.133</v>
+        <v>1092.121</v>
       </c>
       <c r="F554">
         <v>64790.03</v>
@@ -24456,25 +24456,25 @@
         <v>-315.144</v>
       </c>
       <c r="H554">
-        <v>25593.223</v>
+        <v>24902.258</v>
       </c>
       <c r="I554">
-        <v>3460.734</v>
+        <v>3234.951</v>
       </c>
       <c r="J554">
-        <v>1685.532</v>
+        <v>1716.064</v>
       </c>
       <c r="K554">
-        <v>1302.559</v>
+        <v>1274.093</v>
       </c>
       <c r="L554">
-        <v>4037.444</v>
+        <v>3896.414</v>
       </c>
       <c r="M554">
-        <v>23935.68</v>
+        <v>23189.489</v>
       </c>
       <c r="N554">
-        <v>306458.456</v>
+        <v>306894.214</v>
       </c>
     </row>
     <row r="555" spans="1:14">
@@ -24482,16 +24482,16 @@
         <v>43160</v>
       </c>
       <c r="B555">
-        <v>80690.559</v>
+        <v>80625.663</v>
       </c>
       <c r="C555">
-        <v>1413.53</v>
+        <v>1471.84</v>
       </c>
       <c r="D555">
-        <v>103883.887</v>
+        <v>106523.78</v>
       </c>
       <c r="E555">
-        <v>1193.172</v>
+        <v>1158.37</v>
       </c>
       <c r="F555">
         <v>67032.656</v>
@@ -24500,25 +24500,25 @@
         <v>-489.962</v>
       </c>
       <c r="H555">
-        <v>25887.238</v>
+        <v>25860.604</v>
       </c>
       <c r="I555">
-        <v>3629.646</v>
+        <v>3547.442</v>
       </c>
       <c r="J555">
-        <v>1806.108</v>
+        <v>1821.764</v>
       </c>
       <c r="K555">
-        <v>1384.92</v>
+        <v>1366.753</v>
       </c>
       <c r="L555">
-        <v>5099.244</v>
+        <v>5056.238</v>
       </c>
       <c r="M555">
-        <v>27275.001</v>
+        <v>26463.704</v>
       </c>
       <c r="N555">
-        <v>319916.607</v>
+        <v>321546.954</v>
       </c>
     </row>
     <row r="556" spans="1:14">
@@ -24526,43 +24526,43 @@
         <v>43191</v>
       </c>
       <c r="B556">
-        <v>73488.654</v>
+        <v>73346.006</v>
       </c>
       <c r="C556">
-        <v>1445.962</v>
+        <v>1538.279</v>
       </c>
       <c r="D556">
-        <v>100003.613</v>
+        <v>98371.08</v>
       </c>
       <c r="E556">
-        <v>976.098</v>
+        <v>1098.511</v>
       </c>
       <c r="F556">
-        <v>59087.001</v>
+        <v>59133.155</v>
       </c>
       <c r="G556">
         <v>-376.898</v>
       </c>
       <c r="H556">
-        <v>27615.075</v>
+        <v>28115.155</v>
       </c>
       <c r="I556">
-        <v>3163.189</v>
+        <v>3101.87</v>
       </c>
       <c r="J556">
-        <v>1709.409</v>
+        <v>1725.698</v>
       </c>
       <c r="K556">
-        <v>1211.653</v>
+        <v>1187.937</v>
       </c>
       <c r="L556">
-        <v>6111.169</v>
+        <v>6056.727</v>
       </c>
       <c r="M556">
-        <v>26756.676</v>
+        <v>26430.857</v>
       </c>
       <c r="N556">
-        <v>302229.286</v>
+        <v>300756.44</v>
       </c>
     </row>
     <row r="557" spans="1:14">
@@ -24570,16 +24570,16 @@
         <v>43221</v>
       </c>
       <c r="B557">
-        <v>85403.131</v>
+        <v>85227.3</v>
       </c>
       <c r="C557">
-        <v>1449.976</v>
+        <v>1556.805</v>
       </c>
       <c r="D557">
-        <v>115639.447</v>
+        <v>115283.982</v>
       </c>
       <c r="E557">
-        <v>1045.009</v>
+        <v>1167.264</v>
       </c>
       <c r="F557">
         <v>67320.248</v>
@@ -24588,25 +24588,1037 @@
         <v>-390.083</v>
       </c>
       <c r="H557">
-        <v>30291.354</v>
+        <v>30444.284</v>
       </c>
       <c r="I557">
-        <v>3637.235</v>
+        <v>3351.715</v>
       </c>
       <c r="J557">
-        <v>1679.313</v>
+        <v>1731.562</v>
       </c>
       <c r="K557">
-        <v>1408.817</v>
+        <v>1382.62</v>
       </c>
       <c r="L557">
-        <v>7091.272</v>
+        <v>6849.012</v>
       </c>
       <c r="M557">
-        <v>23405.142</v>
+        <v>23953.128</v>
       </c>
       <c r="N557">
-        <v>339055.594</v>
+        <v>338947.606</v>
+      </c>
+    </row>
+    <row r="558" spans="1:14">
+      <c r="A558" s="6">
+        <v>43252</v>
+      </c>
+      <c r="B558">
+        <v>101503.427</v>
+      </c>
+      <c r="C558">
+        <v>1900.568</v>
+      </c>
+      <c r="D558">
+        <v>130826.4</v>
+      </c>
+      <c r="E558">
+        <v>1091.26</v>
+      </c>
+      <c r="F558">
+        <v>69687.556</v>
+      </c>
+      <c r="G558">
+        <v>-433.324</v>
+      </c>
+      <c r="H558">
+        <v>27597.488</v>
+      </c>
+      <c r="I558">
+        <v>3470.749</v>
+      </c>
+      <c r="J558">
+        <v>1719.995</v>
+      </c>
+      <c r="K558">
+        <v>1299.835</v>
+      </c>
+      <c r="L558">
+        <v>7414.667</v>
+      </c>
+      <c r="M558">
+        <v>24702.856</v>
+      </c>
+      <c r="N558">
+        <v>371885.761</v>
+      </c>
+    </row>
+    <row r="559" spans="1:14">
+      <c r="A559" s="6">
+        <v>43282</v>
+      </c>
+      <c r="B559">
+        <v>115376.376</v>
+      </c>
+      <c r="C559">
+        <v>1901.008</v>
+      </c>
+      <c r="D559">
+        <v>164749.06</v>
+      </c>
+      <c r="E559">
+        <v>1171.62</v>
+      </c>
+      <c r="F559">
+        <v>72456.009</v>
+      </c>
+      <c r="G559">
+        <v>-644.469</v>
+      </c>
+      <c r="H559">
+        <v>25099.529</v>
+      </c>
+      <c r="I559">
+        <v>3749.456</v>
+      </c>
+      <c r="J559">
+        <v>1750.031</v>
+      </c>
+      <c r="K559">
+        <v>1369.611</v>
+      </c>
+      <c r="L559">
+        <v>6754.876</v>
+      </c>
+      <c r="M559">
+        <v>16446.574</v>
+      </c>
+      <c r="N559">
+        <v>411290.32</v>
+      </c>
+    </row>
+    <row r="560" spans="1:14">
+      <c r="A560" s="6">
+        <v>43313</v>
+      </c>
+      <c r="B560">
+        <v>115129.456</v>
+      </c>
+      <c r="C560">
+        <v>1926.706</v>
+      </c>
+      <c r="D560">
+        <v>161676.241</v>
+      </c>
+      <c r="E560">
+        <v>1301.002</v>
+      </c>
+      <c r="F560">
+        <v>72282.467</v>
+      </c>
+      <c r="G560">
+        <v>-747.235</v>
+      </c>
+      <c r="H560">
+        <v>22016.905</v>
+      </c>
+      <c r="I560">
+        <v>3629.802</v>
+      </c>
+      <c r="J560">
+        <v>1757.519</v>
+      </c>
+      <c r="K560">
+        <v>1367.055</v>
+      </c>
+      <c r="L560">
+        <v>6695.408</v>
+      </c>
+      <c r="M560">
+        <v>19846.437</v>
+      </c>
+      <c r="N560">
+        <v>408027.757</v>
+      </c>
+    </row>
+    <row r="561" spans="1:14">
+      <c r="A561" s="6">
+        <v>43344</v>
+      </c>
+      <c r="B561">
+        <v>96543.992</v>
+      </c>
+      <c r="C561">
+        <v>1854.029</v>
+      </c>
+      <c r="D561">
+        <v>141785.528</v>
+      </c>
+      <c r="E561">
+        <v>1104.358</v>
+      </c>
+      <c r="F561">
+        <v>64724.753</v>
+      </c>
+      <c r="G561">
+        <v>-603.113</v>
+      </c>
+      <c r="H561">
+        <v>19165.621</v>
+      </c>
+      <c r="I561">
+        <v>3280.616</v>
+      </c>
+      <c r="J561">
+        <v>1589.557</v>
+      </c>
+      <c r="K561">
+        <v>1327.908</v>
+      </c>
+      <c r="L561">
+        <v>5960.901</v>
+      </c>
+      <c r="M561">
+        <v>18519.671</v>
+      </c>
+      <c r="N561">
+        <v>356258.302</v>
+      </c>
+    </row>
+    <row r="562" spans="1:14">
+      <c r="A562" s="6">
+        <v>43374</v>
+      </c>
+      <c r="B562">
+        <v>87263.627</v>
+      </c>
+      <c r="C562">
+        <v>1576.709</v>
+      </c>
+      <c r="D562">
+        <v>123142.239</v>
+      </c>
+      <c r="E562">
+        <v>1016.002</v>
+      </c>
+      <c r="F562">
+        <v>59396.905</v>
+      </c>
+      <c r="G562">
+        <v>-492.202</v>
+      </c>
+      <c r="H562">
+        <v>19548.191</v>
+      </c>
+      <c r="I562">
+        <v>3215.944</v>
+      </c>
+      <c r="J562">
+        <v>1743.386</v>
+      </c>
+      <c r="K562">
+        <v>1273.09</v>
+      </c>
+      <c r="L562">
+        <v>4969.691</v>
+      </c>
+      <c r="M562">
+        <v>21193.898</v>
+      </c>
+      <c r="N562">
+        <v>324931.943</v>
+      </c>
+    </row>
+    <row r="563" spans="1:14">
+      <c r="A563" s="6">
+        <v>43405</v>
+      </c>
+      <c r="B563">
+        <v>92818.594</v>
+      </c>
+      <c r="C563">
+        <v>1661.133</v>
+      </c>
+      <c r="D563">
+        <v>108167.635</v>
+      </c>
+      <c r="E563">
+        <v>1045.119</v>
+      </c>
+      <c r="F563">
+        <v>63954.37</v>
+      </c>
+      <c r="G563">
+        <v>-342.707</v>
+      </c>
+      <c r="H563">
+        <v>21912.716</v>
+      </c>
+      <c r="I563">
+        <v>3263.571</v>
+      </c>
+      <c r="J563">
+        <v>1724.295</v>
+      </c>
+      <c r="K563">
+        <v>1330.844</v>
+      </c>
+      <c r="L563">
+        <v>3742.765</v>
+      </c>
+      <c r="M563">
+        <v>22015.734</v>
+      </c>
+      <c r="N563">
+        <v>322368.657</v>
+      </c>
+    </row>
+    <row r="564" spans="1:14">
+      <c r="A564" s="6">
+        <v>43435</v>
+      </c>
+      <c r="B564">
+        <v>100318.6</v>
+      </c>
+      <c r="C564">
+        <v>1761.02</v>
+      </c>
+      <c r="D564">
+        <v>109801.976</v>
+      </c>
+      <c r="E564">
+        <v>1120.499</v>
+      </c>
+      <c r="F564">
+        <v>71657.288</v>
+      </c>
+      <c r="G564">
+        <v>-522.071</v>
+      </c>
+      <c r="H564">
+        <v>22797.161</v>
+      </c>
+      <c r="I564">
+        <v>3404.054</v>
+      </c>
+      <c r="J564">
+        <v>1799.287</v>
+      </c>
+      <c r="K564">
+        <v>1446.081</v>
+      </c>
+      <c r="L564">
+        <v>3109.64</v>
+      </c>
+      <c r="M564">
+        <v>24306.284</v>
+      </c>
+      <c r="N564">
+        <v>342139.112</v>
+      </c>
+    </row>
+    <row r="565" spans="1:14">
+      <c r="A565" s="6">
+        <v>43466</v>
+      </c>
+      <c r="B565">
+        <v>101007.931</v>
+      </c>
+      <c r="C565">
+        <v>2198.078</v>
+      </c>
+      <c r="D565">
+        <v>119306.715</v>
+      </c>
+      <c r="E565">
+        <v>1114.523</v>
+      </c>
+      <c r="F565">
+        <v>73700.844</v>
+      </c>
+      <c r="G565">
+        <v>-323.009</v>
+      </c>
+      <c r="H565">
+        <v>24209.767</v>
+      </c>
+      <c r="I565">
+        <v>3533.21</v>
+      </c>
+      <c r="J565">
+        <v>1612.458</v>
+      </c>
+      <c r="K565">
+        <v>1421.546</v>
+      </c>
+      <c r="L565">
+        <v>3655.189</v>
+      </c>
+      <c r="M565">
+        <v>25121.684</v>
+      </c>
+      <c r="N565">
+        <v>357753.652</v>
+      </c>
+    </row>
+    <row r="566" spans="1:14">
+      <c r="A566" s="6">
+        <v>43497</v>
+      </c>
+      <c r="B566">
+        <v>80104.492</v>
+      </c>
+      <c r="C566">
+        <v>1552.487</v>
+      </c>
+      <c r="D566">
+        <v>111004.764</v>
+      </c>
+      <c r="E566">
+        <v>1110.37</v>
+      </c>
+      <c r="F566">
+        <v>64714.894</v>
+      </c>
+      <c r="G566">
+        <v>-388.719</v>
+      </c>
+      <c r="H566">
+        <v>21826.166</v>
+      </c>
+      <c r="I566">
+        <v>3165.172</v>
+      </c>
+      <c r="J566">
+        <v>1453.68</v>
+      </c>
+      <c r="K566">
+        <v>1307.982</v>
+      </c>
+      <c r="L566">
+        <v>3826.741</v>
+      </c>
+      <c r="M566">
+        <v>23000.43</v>
+      </c>
+      <c r="N566">
+        <v>313680.416</v>
+      </c>
+    </row>
+    <row r="567" spans="1:14">
+      <c r="A567" s="6">
+        <v>43525</v>
+      </c>
+      <c r="B567">
+        <v>78516.404</v>
+      </c>
+      <c r="C567">
+        <v>1461.997</v>
+      </c>
+      <c r="D567">
+        <v>112945.074</v>
+      </c>
+      <c r="E567">
+        <v>1250.899</v>
+      </c>
+      <c r="F567">
+        <v>65079.691</v>
+      </c>
+      <c r="G567">
+        <v>-408.942</v>
+      </c>
+      <c r="H567">
+        <v>25546.144</v>
+      </c>
+      <c r="I567">
+        <v>3257</v>
+      </c>
+      <c r="J567">
+        <v>1589.539</v>
+      </c>
+      <c r="K567">
+        <v>1437.009</v>
+      </c>
+      <c r="L567">
+        <v>5909.724</v>
+      </c>
+      <c r="M567">
+        <v>26115.747</v>
+      </c>
+      <c r="N567">
+        <v>323782.389</v>
+      </c>
+    </row>
+    <row r="568" spans="1:14">
+      <c r="A568" s="6">
+        <v>43556</v>
+      </c>
+      <c r="B568">
+        <v>60007.704</v>
+      </c>
+      <c r="C568">
+        <v>1234.403</v>
+      </c>
+      <c r="D568">
+        <v>103005.959</v>
+      </c>
+      <c r="E568">
+        <v>1071.032</v>
+      </c>
+      <c r="F568">
+        <v>60580.927</v>
+      </c>
+      <c r="G568">
+        <v>-103.221</v>
+      </c>
+      <c r="H568">
+        <v>25483.404</v>
+      </c>
+      <c r="I568">
+        <v>3027.119</v>
+      </c>
+      <c r="J568">
+        <v>1464.037</v>
+      </c>
+      <c r="K568">
+        <v>1239.036</v>
+      </c>
+      <c r="L568">
+        <v>6835.483</v>
+      </c>
+      <c r="M568">
+        <v>29710.637</v>
+      </c>
+      <c r="N568">
+        <v>294576.767</v>
+      </c>
+    </row>
+    <row r="569" spans="1:14">
+      <c r="A569" s="6">
+        <v>43586</v>
+      </c>
+      <c r="B569">
+        <v>71882.572</v>
+      </c>
+      <c r="C569">
+        <v>1689.977</v>
+      </c>
+      <c r="D569">
+        <v>116236.162</v>
+      </c>
+      <c r="E569">
+        <v>1101.396</v>
+      </c>
+      <c r="F569">
+        <v>67123.546</v>
+      </c>
+      <c r="G569">
+        <v>-368.281</v>
+      </c>
+      <c r="H569">
+        <v>30060.652</v>
+      </c>
+      <c r="I569">
+        <v>3365.113</v>
+      </c>
+      <c r="J569">
+        <v>1541.503</v>
+      </c>
+      <c r="K569">
+        <v>1347.171</v>
+      </c>
+      <c r="L569">
+        <v>7191.398</v>
+      </c>
+      <c r="M569">
+        <v>25973.433</v>
+      </c>
+      <c r="N569">
+        <v>328268.508</v>
+      </c>
+    </row>
+    <row r="570" spans="1:14">
+      <c r="A570" s="6">
+        <v>43617</v>
+      </c>
+      <c r="B570">
+        <v>78609.515</v>
+      </c>
+      <c r="C570">
+        <v>1530.983</v>
+      </c>
+      <c r="D570">
+        <v>136993.984</v>
+      </c>
+      <c r="E570">
+        <v>1025.048</v>
+      </c>
+      <c r="F570">
+        <v>68804.879</v>
+      </c>
+      <c r="G570">
+        <v>-385.296</v>
+      </c>
+      <c r="H570">
+        <v>26468.797</v>
+      </c>
+      <c r="I570">
+        <v>3338.682</v>
+      </c>
+      <c r="J570">
+        <v>1553.75</v>
+      </c>
+      <c r="K570">
+        <v>1362.329</v>
+      </c>
+      <c r="L570">
+        <v>8005.559</v>
+      </c>
+      <c r="M570">
+        <v>22947.492</v>
+      </c>
+      <c r="N570">
+        <v>351362.689</v>
+      </c>
+    </row>
+    <row r="571" spans="1:14">
+      <c r="A571" s="6">
+        <v>43647</v>
+      </c>
+      <c r="B571">
+        <v>100981.204</v>
+      </c>
+      <c r="C571">
+        <v>1775.341</v>
+      </c>
+      <c r="D571">
+        <v>174340.987</v>
+      </c>
+      <c r="E571">
+        <v>1289.984</v>
+      </c>
+      <c r="F571">
+        <v>72198.595</v>
+      </c>
+      <c r="G571">
+        <v>-622.347</v>
+      </c>
+      <c r="H571">
+        <v>23729.755</v>
+      </c>
+      <c r="I571">
+        <v>3569.273</v>
+      </c>
+      <c r="J571">
+        <v>1587.295</v>
+      </c>
+      <c r="K571">
+        <v>1411.632</v>
+      </c>
+      <c r="L571">
+        <v>8168.61</v>
+      </c>
+      <c r="M571">
+        <v>22024.187</v>
+      </c>
+      <c r="N571">
+        <v>411616.143</v>
+      </c>
+    </row>
+    <row r="572" spans="1:14">
+      <c r="A572" s="6">
+        <v>43678</v>
+      </c>
+      <c r="B572">
+        <v>94177.218</v>
+      </c>
+      <c r="C572">
+        <v>1770.818</v>
+      </c>
+      <c r="D572">
+        <v>176457.797</v>
+      </c>
+      <c r="E572">
+        <v>1202.099</v>
+      </c>
+      <c r="F572">
+        <v>71910.684</v>
+      </c>
+      <c r="G572">
+        <v>-579.012</v>
+      </c>
+      <c r="H572">
+        <v>21041.242</v>
+      </c>
+      <c r="I572">
+        <v>3717.001</v>
+      </c>
+      <c r="J572">
+        <v>1601.676</v>
+      </c>
+      <c r="K572">
+        <v>1409.472</v>
+      </c>
+      <c r="L572">
+        <v>7887.784</v>
+      </c>
+      <c r="M572">
+        <v>19869.229</v>
+      </c>
+      <c r="N572">
+        <v>401664.943</v>
+      </c>
+    </row>
+    <row r="573" spans="1:14">
+      <c r="A573" s="6">
+        <v>43709</v>
+      </c>
+      <c r="B573">
+        <v>85918.411</v>
+      </c>
+      <c r="C573">
+        <v>1579.989</v>
+      </c>
+      <c r="D573">
+        <v>150752.719</v>
+      </c>
+      <c r="E573">
+        <v>1138.981</v>
+      </c>
+      <c r="F573">
+        <v>66063.58</v>
+      </c>
+      <c r="G573">
+        <v>-671.214</v>
+      </c>
+      <c r="H573">
+        <v>16323.717</v>
+      </c>
+      <c r="I573">
+        <v>3282.4</v>
+      </c>
+      <c r="J573">
+        <v>1506.084</v>
+      </c>
+      <c r="K573">
+        <v>1384.449</v>
+      </c>
+      <c r="L573">
+        <v>6752.219</v>
+      </c>
+      <c r="M573">
+        <v>24385.394</v>
+      </c>
+      <c r="N573">
+        <v>359545.113</v>
+      </c>
+    </row>
+    <row r="574" spans="1:14">
+      <c r="A574" s="6">
+        <v>43739</v>
+      </c>
+      <c r="B574">
+        <v>66828.543</v>
+      </c>
+      <c r="C574">
+        <v>1152.642</v>
+      </c>
+      <c r="D574">
+        <v>133667.036</v>
+      </c>
+      <c r="E574">
+        <v>997.29</v>
+      </c>
+      <c r="F574">
+        <v>62032.622</v>
+      </c>
+      <c r="G574">
+        <v>-372.614</v>
+      </c>
+      <c r="H574">
+        <v>16291.714</v>
+      </c>
+      <c r="I574">
+        <v>3081.458</v>
+      </c>
+      <c r="J574">
+        <v>1565.47</v>
+      </c>
+      <c r="K574">
+        <v>1276.961</v>
+      </c>
+      <c r="L574">
+        <v>6130.609</v>
+      </c>
+      <c r="M574">
+        <v>28136.358</v>
+      </c>
+      <c r="N574">
+        <v>321874.964</v>
+      </c>
+    </row>
+    <row r="575" spans="1:14">
+      <c r="A575" s="6">
+        <v>43770</v>
+      </c>
+      <c r="B575">
+        <v>75560.454</v>
+      </c>
+      <c r="C575">
+        <v>1249.966</v>
+      </c>
+      <c r="D575">
+        <v>117762.159</v>
+      </c>
+      <c r="E575">
+        <v>1196.105</v>
+      </c>
+      <c r="F575">
+        <v>64125.425</v>
+      </c>
+      <c r="G575">
+        <v>-508.775</v>
+      </c>
+      <c r="H575">
+        <v>20519.976</v>
+      </c>
+      <c r="I575">
+        <v>3106.903</v>
+      </c>
+      <c r="J575">
+        <v>1497.456</v>
+      </c>
+      <c r="K575">
+        <v>1111.654</v>
+      </c>
+      <c r="L575">
+        <v>4376.6</v>
+      </c>
+      <c r="M575">
+        <v>25603.482</v>
+      </c>
+      <c r="N575">
+        <v>316671.897</v>
+      </c>
+    </row>
+    <row r="576" spans="1:14">
+      <c r="A576" s="6">
+        <v>43800</v>
+      </c>
+      <c r="B576">
+        <v>72553.902</v>
+      </c>
+      <c r="C576">
+        <v>1370.231</v>
+      </c>
+      <c r="D576">
+        <v>129341.72</v>
+      </c>
+      <c r="E576">
+        <v>1136.387</v>
+      </c>
+      <c r="F576">
+        <v>73073.575</v>
+      </c>
+      <c r="G576">
+        <v>-529.314</v>
+      </c>
+      <c r="H576">
+        <v>22206.034</v>
+      </c>
+      <c r="I576">
+        <v>3407.44</v>
+      </c>
+      <c r="J576">
+        <v>1588.443</v>
+      </c>
+      <c r="K576">
+        <v>1301.345</v>
+      </c>
+      <c r="L576">
+        <v>3494.258</v>
+      </c>
+      <c r="M576">
+        <v>27182.955</v>
+      </c>
+      <c r="N576">
+        <v>337253.095</v>
+      </c>
+    </row>
+    <row r="577" spans="1:14">
+      <c r="A577" s="6">
+        <v>43831</v>
+      </c>
+      <c r="B577">
+        <v>65170.388</v>
+      </c>
+      <c r="C577">
+        <v>1620.092</v>
+      </c>
+      <c r="D577">
+        <v>132980.029</v>
+      </c>
+      <c r="E577">
+        <v>1210.667</v>
+      </c>
+      <c r="F577">
+        <v>74204.038</v>
+      </c>
+      <c r="G577">
+        <v>-406.027</v>
+      </c>
+      <c r="H577">
+        <v>24286.316</v>
+      </c>
+      <c r="I577">
+        <v>3348.534</v>
+      </c>
+      <c r="J577">
+        <v>1608.71</v>
+      </c>
+      <c r="K577">
+        <v>1255.173</v>
+      </c>
+      <c r="L577">
+        <v>4554.754</v>
+      </c>
+      <c r="M577">
+        <v>28403.342</v>
+      </c>
+      <c r="N577">
+        <v>339320.359</v>
+      </c>
+    </row>
+    <row r="578" spans="1:14">
+      <c r="A578" s="6">
+        <v>43862</v>
+      </c>
+      <c r="B578">
+        <v>56071.592</v>
+      </c>
+      <c r="C578">
+        <v>1201.763</v>
+      </c>
+      <c r="D578">
+        <v>126023.646</v>
+      </c>
+      <c r="E578">
+        <v>1233.506</v>
+      </c>
+      <c r="F578">
+        <v>65950.342</v>
+      </c>
+      <c r="G578">
+        <v>-246.677</v>
+      </c>
+      <c r="H578">
+        <v>25076.89</v>
+      </c>
+      <c r="I578">
+        <v>3154.205</v>
+      </c>
+      <c r="J578">
+        <v>1460.893</v>
+      </c>
+      <c r="K578">
+        <v>1155.821</v>
+      </c>
+      <c r="L578">
+        <v>5651.852</v>
+      </c>
+      <c r="M578">
+        <v>29234.788</v>
+      </c>
+      <c r="N578">
+        <v>316934.16</v>
+      </c>
+    </row>
+    <row r="579" spans="1:14">
+      <c r="A579" s="6">
+        <v>43891</v>
+      </c>
+      <c r="B579">
+        <v>50585.693</v>
+      </c>
+      <c r="C579">
+        <v>1411.864</v>
+      </c>
+      <c r="D579">
+        <v>123569.382</v>
+      </c>
+      <c r="E579">
+        <v>1109.385</v>
+      </c>
+      <c r="F579">
+        <v>63997.21</v>
+      </c>
+      <c r="G579">
+        <v>-353.064</v>
+      </c>
+      <c r="H579">
+        <v>22269.269</v>
+      </c>
+      <c r="I579">
+        <v>3223.326</v>
+      </c>
+      <c r="J579">
+        <v>1619.886</v>
+      </c>
+      <c r="K579">
+        <v>1490.301</v>
+      </c>
+      <c r="L579">
+        <v>6313.841</v>
+      </c>
+      <c r="M579">
+        <v>29483.348</v>
+      </c>
+      <c r="N579">
+        <v>305778.64</v>
+      </c>
+    </row>
+    <row r="580" spans="1:14">
+      <c r="A580" s="6">
+        <v>43922</v>
+      </c>
+      <c r="B580">
+        <v>40575.703</v>
+      </c>
+      <c r="C580">
+        <v>1249.407</v>
+      </c>
+      <c r="D580">
+        <v>108137.502</v>
+      </c>
+      <c r="E580">
+        <v>801.021</v>
+      </c>
+      <c r="F580">
+        <v>59170.016</v>
+      </c>
+      <c r="G580">
+        <v>-325.03</v>
+      </c>
+      <c r="H580">
+        <v>20770.965</v>
+      </c>
+      <c r="I580">
+        <v>2992.197</v>
+      </c>
+      <c r="J580">
+        <v>1531.601</v>
+      </c>
+      <c r="K580">
+        <v>1356.354</v>
+      </c>
+      <c r="L580">
+        <v>8009.763</v>
+      </c>
+      <c r="M580">
+        <v>29534.418</v>
+      </c>
+      <c r="N580">
+        <v>274875.653</v>
       </c>
     </row>
   </sheetData>
@@ -24633,7 +25645,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N81"/>
+  <dimension ref="A1:N83"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A13" sqref="A13"/>
@@ -24654,7 +25666,7 @@
     <col min="11" max="11" width="59.842529" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="54.558105" bestFit="true" customWidth="true" style="0"/>
     <col min="13" max="13" width="53.415527" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="49.130859" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="86.693115" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -27771,16 +28783,16 @@
         <v>2017</v>
       </c>
       <c r="B81">
-        <v>1207901.306</v>
+        <v>1205835.276</v>
       </c>
       <c r="C81">
-        <v>21091.171</v>
+        <v>21389.945</v>
       </c>
       <c r="D81">
-        <v>1272864.166</v>
+        <v>1296442.491</v>
       </c>
       <c r="E81">
-        <v>14158.866</v>
+        <v>12468.967</v>
       </c>
       <c r="F81">
         <v>804949.635</v>
@@ -27789,25 +28801,113 @@
         <v>-6494.548</v>
       </c>
       <c r="H81">
-        <v>300044.503</v>
+        <v>300332.93</v>
       </c>
       <c r="I81">
-        <v>43283.917</v>
+        <v>41123.518</v>
       </c>
       <c r="J81">
-        <v>20772.616</v>
+        <v>21609.894</v>
       </c>
       <c r="K81">
-        <v>15976.041</v>
+        <v>15926.774</v>
       </c>
       <c r="L81">
-        <v>52957.779</v>
+        <v>53286.865</v>
       </c>
       <c r="M81">
-        <v>254254.339</v>
+        <v>254302.695</v>
       </c>
       <c r="N81">
-        <v>4014804.462</v>
+        <v>4034270.559</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14">
+      <c r="A82" s="7">
+        <v>2018</v>
+      </c>
+      <c r="B82">
+        <v>1149487.339</v>
+      </c>
+      <c r="C82">
+        <v>25225.618</v>
+      </c>
+      <c r="D82">
+        <v>1469132.682</v>
+      </c>
+      <c r="E82">
+        <v>13462.749</v>
+      </c>
+      <c r="F82">
+        <v>807084.477</v>
+      </c>
+      <c r="G82">
+        <v>-5904.539</v>
+      </c>
+      <c r="H82">
+        <v>292523.989</v>
+      </c>
+      <c r="I82">
+        <v>40936.159</v>
+      </c>
+      <c r="J82">
+        <v>20895.765</v>
+      </c>
+      <c r="K82">
+        <v>15967.134</v>
+      </c>
+      <c r="L82">
+        <v>63825.315</v>
+      </c>
+      <c r="M82">
+        <v>272667.454</v>
+      </c>
+      <c r="N82">
+        <v>4178277.344</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14">
+      <c r="A83" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B83">
+        <v>966148.35</v>
+      </c>
+      <c r="C83">
+        <v>18566.912</v>
+      </c>
+      <c r="D83">
+        <v>1581815.076</v>
+      </c>
+      <c r="E83">
+        <v>13634.113</v>
+      </c>
+      <c r="F83">
+        <v>809409.262</v>
+      </c>
+      <c r="G83">
+        <v>-5260.744</v>
+      </c>
+      <c r="H83">
+        <v>273707.366</v>
+      </c>
+      <c r="I83">
+        <v>39850.771</v>
+      </c>
+      <c r="J83">
+        <v>18561.39</v>
+      </c>
+      <c r="K83">
+        <v>16010.586</v>
+      </c>
+      <c r="L83">
+        <v>72234.174</v>
+      </c>
+      <c r="M83">
+        <v>300071.029</v>
+      </c>
+      <c r="N83">
+        <v>4118050.576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to latest release
</commit_message>
<xml_diff>
--- a/data/Table_7.2a_Electricity_Net_Generation__Total_(All_Sectors).xlsx
+++ b/data/Table_7.2a_Electricity_Net_Generation__Total_(All_Sectors).xlsx
@@ -21,13 +21,13 @@
     <t>U.S. Energy Information Administration</t>
   </si>
   <si>
-    <t>July 2020 Monthly Energy Review</t>
+    <t>August 2020 Monthly Energy Review</t>
   </si>
   <si>
-    <t>Release Date: July 28, 2020</t>
+    <t>Release Date: August 26, 2020</t>
   </si>
   <si>
-    <t>Next Update: August 26, 2020</t>
+    <t>Next Update: September 24, 2020</t>
   </si>
   <si>
     <t>Table 7.2a Electricity Net Generation: Total (All Sectors)</t>
@@ -488,7 +488,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N580"/>
+  <dimension ref="A1:N581"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A13" sqref="A13"/>
@@ -25619,6 +25619,50 @@
       </c>
       <c r="N580">
         <v>274875.653</v>
+      </c>
+    </row>
+    <row r="581" spans="1:14">
+      <c r="A581" s="6">
+        <v>43952</v>
+      </c>
+      <c r="B581">
+        <v>46488.016</v>
+      </c>
+      <c r="C581">
+        <v>1325.726</v>
+      </c>
+      <c r="D581">
+        <v>116235.595</v>
+      </c>
+      <c r="E581">
+        <v>862.426</v>
+      </c>
+      <c r="F581">
+        <v>64337.97</v>
+      </c>
+      <c r="G581">
+        <v>-366.733</v>
+      </c>
+      <c r="H581">
+        <v>29467.557</v>
+      </c>
+      <c r="I581">
+        <v>3103.467</v>
+      </c>
+      <c r="J581">
+        <v>1550.451</v>
+      </c>
+      <c r="K581">
+        <v>1420.599</v>
+      </c>
+      <c r="L581">
+        <v>9741.524</v>
+      </c>
+      <c r="M581">
+        <v>28180.321</v>
+      </c>
+      <c r="N581">
+        <v>303434.419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>